<commit_message>
Update to assignment tracking doc, minutes from meeting added
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EA14EC-4016-441B-B1BE-837D27338DBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEFA741-C9A9-4D7F-AFC2-BF27F28AFCAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Refer to RMIT Easy Cite tool for examples</t>
-  </si>
-  <si>
-    <t>Submission: 1 file via Turnitin</t>
   </si>
   <si>
     <t>https://leevdb.github.io/Lee-van-den-Blink/</t>
@@ -233,12 +230,6 @@
     <t>in the report</t>
   </si>
   <si>
-    <t>not sure whats on website yet</t>
-  </si>
-  <si>
-    <t>WEBSITE</t>
-  </si>
-  <si>
     <t>included in report</t>
   </si>
   <si>
@@ -331,7 +322,19 @@
     <t>refer rubric</t>
   </si>
   <si>
-    <t>? Github?  Not sure whats supposed to be on the github website?</t>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>to do at the end</t>
+  </si>
+  <si>
+    <t>X (with assistance)</t>
+  </si>
+  <si>
+    <t>clarify this s needed.</t>
+  </si>
+  <si>
+    <t>Submission: 1 file</t>
   </si>
 </sst>
 </file>
@@ -934,8 +937,8 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -962,7 +965,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>21</v>
@@ -993,17 +996,17 @@
         <v>9</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1023,7 +1026,7 @@
     </row>
     <row r="3" spans="1:26" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1031,17 +1034,17 @@
         <v>10</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1069,17 +1072,17 @@
         <v>11</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1107,17 +1110,17 @@
         <v>13</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K5" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="6" spans="1:26" ht="12.75">
       <c r="A6" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1145,17 +1148,17 @@
         <v>12</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1181,17 +1184,17 @@
         <v>14</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1304,7 +1307,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="2"/>
@@ -1338,9 +1341,11 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
-      <c r="K11" s="36"/>
+      <c r="K11" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1359,11 +1364,11 @@
     </row>
     <row r="12" spans="1:26" ht="51">
       <c r="A12" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1391,20 +1396,22 @@
     </row>
     <row r="13" spans="1:26" ht="114.75">
       <c r="A13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="I13" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="J13" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" s="36"/>
       <c r="L13" s="2"/>
@@ -1466,7 +1473,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="2"/>
@@ -1487,21 +1494,17 @@
     </row>
     <row r="16" spans="1:26" ht="12.75">
       <c r="A16" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="13" t="s">
-        <v>68</v>
-      </c>
+      <c r="C16" s="13"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="34" t="s">
-        <v>69</v>
-      </c>
+      <c r="J16" s="34"/>
       <c r="K16" s="36"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1521,10 +1524,12 @@
     </row>
     <row r="17" spans="1:26" ht="25.5">
       <c r="A17" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
+      <c r="C17" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1532,7 +1537,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K17" s="36"/>
       <c r="L17" s="2"/>
@@ -1553,11 +1558,11 @@
     </row>
     <row r="18" spans="1:26" ht="51">
       <c r="A18" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -1566,7 +1571,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K18" s="36"/>
       <c r="L18" s="2"/>
@@ -1615,7 +1620,7 @@
     </row>
     <row r="20" spans="1:26" ht="12.75">
       <c r="A20" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" s="22">
         <v>0.5</v>
@@ -1628,7 +1633,7 @@
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
       <c r="J20" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="2"/>
@@ -1647,16 +1652,18 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="30">
+    <row r="21" spans="1:26" ht="15">
       <c r="A21" s="46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
@@ -1681,14 +1688,16 @@
     </row>
     <row r="22" spans="1:26" ht="38.25">
       <c r="A22" s="46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -1713,14 +1722,16 @@
     </row>
     <row r="23" spans="1:26" ht="25.5">
       <c r="A23" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="E23" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -1745,13 +1756,15 @@
     </row>
     <row r="24" spans="1:26" ht="38.25">
       <c r="A24" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -1777,11 +1790,11 @@
     </row>
     <row r="25" spans="1:26" ht="25.5">
       <c r="A25" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
@@ -1809,17 +1822,19 @@
     </row>
     <row r="26" spans="1:26" ht="102">
       <c r="A26" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="H26" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="36"/>
@@ -1841,17 +1856,19 @@
     </row>
     <row r="27" spans="1:26" ht="25.5">
       <c r="A27" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="H27" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="36"/>
@@ -1873,15 +1890,19 @@
     </row>
     <row r="28" spans="1:26" ht="25.5">
       <c r="A28" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
-      <c r="D28" s="15"/>
+      <c r="D28" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
+      <c r="F28" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -1905,15 +1926,17 @@
     </row>
     <row r="29" spans="1:26" ht="12.75">
       <c r="A29" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -1937,11 +1960,11 @@
     </row>
     <row r="30" spans="1:26" ht="38.25">
       <c r="A30" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -2025,7 +2048,7 @@
     </row>
     <row r="33" spans="1:26" ht="12.75">
       <c r="A33" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="22">
         <v>0.1</v>
@@ -2038,7 +2061,7 @@
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
       <c r="J33" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K33" s="10"/>
       <c r="L33" s="2"/>
@@ -2059,16 +2082,18 @@
     </row>
     <row r="34" spans="1:26" ht="25.5">
       <c r="A34" s="37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="G34" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
@@ -2179,11 +2204,11 @@
     </row>
     <row r="38" spans="1:26" ht="25.5">
       <c r="A38" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>20</v>
@@ -2283,11 +2308,11 @@
     </row>
     <row r="41" spans="1:26" ht="12.75">
       <c r="A41" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>20</v>
@@ -2327,10 +2352,12 @@
     </row>
     <row r="42" spans="1:26" ht="12.75">
       <c r="A42" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="C42" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="D42" s="15" t="s">
         <v>20</v>
       </c>
@@ -2691,11 +2718,11 @@
     </row>
     <row r="54" spans="1:26" ht="12.75">
       <c r="A54" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2725,7 +2752,7 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2755,7 +2782,7 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>

</xml_diff>

<commit_message>
Group Processes added to project description doc, assignment tracker updated
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EBECF4-2054-43E4-B15E-C5A93F424E56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E247344-E2E5-4F20-AF7C-1BE5405FC086}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -335,12 +335,21 @@
   <si>
     <t>Submission: 1 file</t>
   </si>
+  <si>
+    <t>overview &amp; Motivation sections completed</t>
+  </si>
+  <si>
+    <t>drafted</t>
+  </si>
+  <si>
+    <t>DRAFT COMPLETE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -439,8 +448,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +504,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -513,11 +534,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -608,7 +630,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -617,8 +638,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,8 +962,8 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1141,7 +1164,7 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="12.75">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="2"/>
@@ -1372,7 +1395,7 @@
       <c r="C12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="47" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="14"/>
@@ -1656,8 +1679,8 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="15">
-      <c r="A21" s="46" t="s">
+    <row r="21" spans="1:26" ht="30">
+      <c r="A21" s="45" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="12"/>
@@ -1672,7 +1695,9 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="J21" s="15" t="s">
+        <v>102</v>
+      </c>
       <c r="K21" s="36"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1691,7 +1716,7 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="38.25">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="45" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="12"/>
@@ -1725,7 +1750,7 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="25.5">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>74</v>
       </c>
       <c r="B23" s="12"/>
@@ -1910,7 +1935,9 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="J28" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="K28" s="36"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1928,7 +1955,7 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" spans="1:26" ht="12.75">
+    <row r="29" spans="1:26" ht="15">
       <c r="A29" s="11" t="s">
         <v>85</v>
       </c>
@@ -1938,14 +1965,16 @@
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="48" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="36"/>
+      <c r="K29" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1970,14 +1999,18 @@
       <c r="C30" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="48" t="s">
+        <v>20</v>
+      </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="36"/>
+      <c r="K30" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -2005,7 +2038,7 @@
       <c r="H31" s="43"/>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
-      <c r="K31" s="44"/>
+      <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2381,7 +2414,7 @@
         <v>20</v>
       </c>
       <c r="J42" s="11"/>
-      <c r="K42" s="47"/>
+      <c r="K42" s="46"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>

</xml_diff>

<commit_message>
Minutes added for 280419, updated tracking doc
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E247344-E2E5-4F20-AF7C-1BE5405FC086}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C478847-5037-4FC5-B4F4-23306AB36177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -344,6 +344,18 @@
   <si>
     <t>DRAFT COMPLETE</t>
   </si>
+  <si>
+    <t>Presentation 5</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>voiceover</t>
+  </si>
+  <si>
+    <t>Nathan working on draft script and presentation for next week.</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +521,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -541,7 +559,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -639,6 +657,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="4" builtinId="26"/>
@@ -962,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1825,7 +1844,9 @@
       <c r="C25" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -2128,13 +2149,15 @@
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="49" t="s">
         <v>20</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
+      <c r="K34" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2902,7 +2925,9 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="12.75">
-      <c r="A59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2930,9 +2955,13 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="12.75">
-      <c r="A60" s="2"/>
+      <c r="A60" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -2958,7 +2987,9 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="12.75">
-      <c r="A61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>

</xml_diff>

<commit_message>
updated timframe, format presentation doc, updated tracking doc with current notes
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C478847-5037-4FC5-B4F4-23306AB36177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20BBA60-A13F-45BE-9877-F9791A4E32B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Nathan working on draft script and presentation for next week.</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>just need harrison role.</t>
   </si>
 </sst>
 </file>
@@ -981,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1698,7 +1704,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="30">
+    <row r="21" spans="1:26" ht="15">
       <c r="A21" s="45" t="s">
         <v>70</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="15"/>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="48" t="s">
         <v>20</v>
       </c>
       <c r="F21" s="15"/>
@@ -1717,7 +1723,9 @@
       <c r="J21" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="K21" s="36"/>
+      <c r="K21" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1743,7 +1751,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="15"/>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="48" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="15"/>
@@ -1751,7 +1759,9 @@
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="36"/>
+      <c r="K22" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1810,7 +1820,7 @@
       <c r="C24" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="48" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="15"/>
@@ -1818,7 +1828,9 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="K24" s="36"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1947,7 +1959,7 @@
         <v>86</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15" t="s">

</xml_diff>

<commit_message>
Updated project description, added timeframe and sound design sections.
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20BBA60-A13F-45BE-9877-F9791A4E32B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABE245A-72DC-4858-9B70-89F9396654AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,18 @@
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="110">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -342,9 +349,6 @@
     <t>drafted</t>
   </si>
   <si>
-    <t>DRAFT COMPLETE</t>
-  </si>
-  <si>
     <t>Presentation 5</t>
   </si>
   <si>
@@ -360,7 +364,7 @@
     <t>I</t>
   </si>
   <si>
-    <t>just need harrison role.</t>
+    <t>Cory has drafts complete just need to push to git</t>
   </si>
 </sst>
 </file>
@@ -987,8 +991,8 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1828,10 +1832,10 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="15" t="s">
-        <v>110</v>
+      <c r="J24" s="15"/>
+      <c r="K24" s="36" t="s">
+        <v>97</v>
       </c>
-      <c r="K24" s="36"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1898,7 +1902,9 @@
         <v>20</v>
       </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="K26" s="36"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1932,7 +1938,9 @@
         <v>20</v>
       </c>
       <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
+      <c r="J27" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="K27" s="36"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1959,10 +1967,10 @@
         <v>86</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E28" s="15"/>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="48" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="15"/>
@@ -1971,7 +1979,9 @@
       <c r="J28" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="K28" s="36"/>
+      <c r="K28" s="36" t="s">
+        <v>97</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -2006,7 +2016,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="36" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2042,7 +2052,7 @@
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="36" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2938,7 +2948,7 @@
     </row>
     <row r="59" spans="1:26" ht="12.75">
       <c r="A59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2968,11 +2978,11 @@
     </row>
     <row r="60" spans="1:26" ht="12.75">
       <c r="A60" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -3000,7 +3010,7 @@
     </row>
     <row r="61" spans="1:26" ht="12.75">
       <c r="A61" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>

</xml_diff>

<commit_message>
Updated presentation doc (my reflection, scope section
Proof read main game doc section, added Nicks object dev and images, group descrptions sections in doc updated.
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABE245A-72DC-4858-9B70-89F9396654AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36A9C9A-1F1A-4B13-866C-DC0EDFBA7847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Group Processes and Communication</t>
   </si>
   <si>
-    <t>Describe communication strategies for group. - minimum 1 paragraph.  Whatis the minimum requirement for communication.</t>
-  </si>
-  <si>
     <t>Skills required, technical experise, etc.</t>
   </si>
   <si>
@@ -361,10 +358,10 @@
     <t>Nathan working on draft script and presentation for next week.</t>
   </si>
   <si>
-    <t>I</t>
+    <t>Cory has drafts complete just need to push to git</t>
   </si>
   <si>
-    <t>Cory has drafts complete just need to push to git</t>
+    <t>:</t>
   </si>
 </sst>
 </file>
@@ -478,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,12 +528,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -569,7 +560,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -598,7 +589,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -662,12 +652,12 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="4" builtinId="26"/>
@@ -992,7 +982,8 @@
   <dimension ref="A1:Z1033"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <pane ySplit="9" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1018,10 +1009,10 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="2"/>
@@ -1046,20 +1037,20 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="32" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="2"/>
@@ -1084,20 +1075,20 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="32" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="2"/>
@@ -1122,17 +1113,17 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="32" t="s">
         <v>42</v>
       </c>
       <c r="K4" t="s">
@@ -1160,20 +1151,20 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="32" t="s">
         <v>48</v>
       </c>
       <c r="L5" s="2"/>
@@ -1193,25 +1184,25 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="12.75">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="34" t="s">
         <v>43</v>
       </c>
       <c r="L6" s="2"/>
@@ -1231,20 +1222,20 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12.75">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="32" t="s">
         <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1397,8 +1388,8 @@
       <c r="J11" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="36" t="s">
-        <v>97</v>
+      <c r="K11" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1424,7 +1415,7 @@
       <c r="C12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="45" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="14"/>
@@ -1433,7 +1424,9 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="36"/>
+      <c r="K12" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1466,10 +1459,10 @@
       <c r="I13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="47"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1487,15 +1480,15 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="12.75">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1515,13 +1508,13 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="12.75">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="21">
         <v>0.05</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1560,8 +1553,10 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="36"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1584,7 +1579,7 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -1595,7 +1590,7 @@
       <c r="J17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="36"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1629,7 +1624,9 @@
       <c r="J18" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="36"/>
+      <c r="K18" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1647,9 +1644,9 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="12.75">
-      <c r="A19" s="24"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1675,19 +1672,19 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="12.75">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <v>0.5</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="9" t="s">
         <v>50</v>
       </c>
@@ -1709,15 +1706,15 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="15">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>71</v>
       </c>
       <c r="D21" s="15"/>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="46" t="s">
         <v>20</v>
       </c>
       <c r="F21" s="15"/>
@@ -1725,10 +1722,10 @@
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
-      <c r="K21" s="36" t="s">
-        <v>97</v>
+      <c r="K21" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1747,15 +1744,15 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="38.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="44" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>73</v>
       </c>
       <c r="D22" s="15"/>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="46" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="15"/>
@@ -1763,8 +1760,8 @@
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="36" t="s">
-        <v>97</v>
+      <c r="K22" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1783,23 +1780,23 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="25.5">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>74</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>75</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="36"/>
+      <c r="K23" s="35"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1821,10 +1818,10 @@
         <v>76</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="15"/>
@@ -1833,8 +1830,8 @@
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="36" t="s">
-        <v>97</v>
+      <c r="K24" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1857,10 +1854,10 @@
         <v>78</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="15"/>
@@ -1869,7 +1866,9 @@
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="36"/>
+      <c r="K25" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1891,7 +1890,7 @@
         <v>80</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>81</v>
       </c>
       <c r="D26" s="15"/>
@@ -1902,10 +1901,10 @@
         <v>20</v>
       </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
-        <v>109</v>
+      <c r="J26" s="36" t="s">
+        <v>107</v>
       </c>
-      <c r="K26" s="36"/>
+      <c r="K26" s="35"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1922,26 +1921,30 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" ht="25.5">
+    <row r="27" spans="1:26" ht="26.25">
       <c r="A27" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="12"/>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="46" t="s">
+        <v>20</v>
+      </c>
       <c r="H27" s="15" t="s">
         <v>20</v>
       </c>
       <c r="I27" s="15"/>
-      <c r="J27" s="15" t="s">
-        <v>109</v>
+      <c r="J27" s="36" t="s">
+        <v>107</v>
       </c>
-      <c r="K27" s="36"/>
+      <c r="K27" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1963,24 +1966,24 @@
         <v>84</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>108</v>
+      <c r="D28" s="46" t="s">
+        <v>20</v>
       </c>
       <c r="E28" s="15"/>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="46" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="K28" s="36" t="s">
-        <v>97</v>
+      <c r="K28" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2003,20 +2006,20 @@
         <v>85</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="24" t="s">
         <v>87</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="46" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="36" t="s">
-        <v>97</v>
+      <c r="K29" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2034,15 +2037,15 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" ht="38.25">
+    <row r="30" spans="1:26" ht="15">
       <c r="A30" s="11" t="s">
         <v>88</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="25" t="s">
-        <v>89</v>
+      <c r="C30" s="24" t="s">
+        <v>108</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="15"/>
@@ -2051,8 +2054,8 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="36" t="s">
-        <v>97</v>
+      <c r="K30" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2071,16 +2074,16 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="12.75">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2099,9 +2102,9 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="12.75">
-      <c r="A32" s="24"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -2127,19 +2130,19 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="12.75">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="21">
         <v>0.1</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="9" t="s">
         <v>50</v>
       </c>
@@ -2160,25 +2163,25 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="25.5">
-      <c r="A34" s="37" t="s">
-        <v>91</v>
+    <row r="34" spans="1:26" ht="26.25">
+      <c r="A34" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="49" t="s">
+      <c r="G34" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="15" t="s">
-        <v>97</v>
+      <c r="K34" s="35" t="s">
+        <v>96</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -2197,9 +2200,9 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="12.75">
-      <c r="A35" s="24"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2225,9 +2228,9 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="12.75">
-      <c r="A36" s="24"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -2253,13 +2256,13 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="12.75">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B37" s="25">
         <v>0.1</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2286,32 +2289,32 @@
     </row>
     <row r="38" spans="1:26" ht="25.5">
       <c r="A38" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="46" t="s">
         <v>20</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H38" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="I38" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="38"/>
-      <c r="K38" s="16"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="47"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2329,9 +2332,9 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" spans="1:26" ht="12.75">
-      <c r="A39" s="24"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -2357,13 +2360,13 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="12.75">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B40" s="25">
         <v>0.1</v>
       </c>
-      <c r="C40" s="21"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2371,7 +2374,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="9"/>
-      <c r="K40" s="39"/>
+      <c r="K40" s="38"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -2388,24 +2391,24 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" spans="1:26" ht="12.75">
+    <row r="41" spans="1:26" ht="15">
       <c r="A41" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="46" t="s">
         <v>20</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H41" s="15" t="s">
@@ -2414,8 +2417,8 @@
       <c r="I41" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="27"/>
-      <c r="K41" s="16"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="47"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2432,13 +2435,13 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" spans="1:26" ht="12.75">
+    <row r="42" spans="1:26" ht="15">
       <c r="A42" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>20</v>
@@ -2459,7 +2462,7 @@
         <v>20</v>
       </c>
       <c r="J42" s="11"/>
-      <c r="K42" s="46"/>
+      <c r="K42" s="48"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2477,16 +2480,16 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="12.75">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -2508,7 +2511,7 @@
       <c r="A44" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="27">
         <v>0.1</v>
       </c>
       <c r="C44" s="7"/>
@@ -2536,7 +2539,7 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" spans="1:26" ht="12.75">
+    <row r="45" spans="1:26" ht="15">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -2546,8 +2549,8 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="16"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="47"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -2593,19 +2596,19 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="12.75">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -2800,7 +2803,7 @@
     </row>
     <row r="54" spans="1:26" ht="12.75">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
@@ -2948,7 +2951,7 @@
     </row>
     <row r="59" spans="1:26" ht="12.75">
       <c r="A59" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2978,11 +2981,11 @@
     </row>
     <row r="60" spans="1:26" ht="12.75">
       <c r="A60" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -3010,7 +3013,7 @@
     </row>
     <row r="61" spans="1:26" ht="12.75">
       <c r="A61" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>

</xml_diff>

<commit_message>
minor update to tracking doc
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36A9C9A-1F1A-4B13-866C-DC0EDFBA7847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA616A-6237-43AA-BC8C-BE86F7D9DF99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Track" sheetId="1" r:id="rId1"/>
@@ -982,7 +982,7 @@
   <dimension ref="A1:Z1033"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -1705,7 +1705,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="15">
+    <row r="21" spans="1:26" ht="30">
       <c r="A21" s="44" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
project description formatting, added career plan bit
</commit_message>
<xml_diff>
--- a/Assignment 3 Tracking - Group 14.xlsx
+++ b/Assignment 3 Tracking - Group 14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CA616A-6237-43AA-BC8C-BE86F7D9DF99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47E49F7-8432-491B-9112-70CB3C3A3CC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -560,7 +560,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -657,7 +657,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="4" builtinId="26"/>
@@ -981,9 +980,9 @@
   </sheetPr>
   <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K42" sqref="K41:K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1462,7 +1461,9 @@
       <c r="J13" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K13" s="47"/>
+      <c r="K13" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1590,7 +1591,9 @@
       <c r="J17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1705,7 +1708,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="30">
+    <row r="21" spans="1:26" ht="15">
       <c r="A21" s="44" t="s">
         <v>70</v>
       </c>
@@ -1796,7 +1799,9 @@
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="35"/>
+      <c r="K23" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1904,7 +1909,9 @@
       <c r="J26" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="35"/>
+      <c r="K26" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2405,20 +2412,22 @@
       <c r="E41" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="46" t="s">
         <v>20</v>
       </c>
       <c r="G41" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="46" t="s">
         <v>20</v>
       </c>
       <c r="J41" s="26"/>
-      <c r="K41" s="47"/>
+      <c r="K41" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2443,26 +2452,28 @@
       <c r="C42" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I42" s="46" t="s">
         <v>20</v>
       </c>
       <c r="J42" s="11"/>
-      <c r="K42" s="48"/>
+      <c r="K42" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>

</xml_diff>